<commit_message>
data from the 2nd experiment is in!
</commit_message>
<xml_diff>
--- a/experiment/results/experiment_1/results_zscored.xlsx
+++ b/experiment/results/experiment_1/results_zscored.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="1220" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="2280" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -526,8 +526,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -711,7 +717,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -799,6 +805,9 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -886,6 +895,9 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1218,7 +1230,7 @@
   <dimension ref="A1:CY137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:CW34"/>
+      <selection activeCell="B5" sqref="B5:CW5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>